<commit_message>
Added code to read data from BME280
</commit_message>
<xml_diff>
--- a/Resources/accel_vals.xlsx
+++ b/Resources/accel_vals.xlsx
@@ -94,6 +94,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -115,6 +116,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -159,16 +161,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -295,10 +301,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S10" activeCellId="0" sqref="S10"/>
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -309,89 +315,89 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="n">
+      <c r="B2" s="3" t="n">
         <v>190</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="n">
+      <c r="E2" s="3" t="n">
         <v>110</v>
       </c>
-      <c r="F2" s="2" t="n">
+      <c r="F2" s="3" t="n">
         <v>180</v>
       </c>
-      <c r="G2" s="2" t="n">
+      <c r="G2" s="3" t="n">
         <v>110</v>
       </c>
-      <c r="H2" s="2" t="n">
+      <c r="H2" s="3" t="n">
         <v>220</v>
       </c>
-      <c r="I2" s="2" t="n">
+      <c r="I2" s="3" t="n">
         <v>160</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="2" t="n">
+      <c r="F3" s="3" t="n">
         <v>60</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="2" t="n">
+      <c r="H3" s="3" t="n">
         <v>170</v>
       </c>
-      <c r="I3" s="2" t="n">
+      <c r="I3" s="3" t="n">
         <v>140</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="3" t="s">
         <v>17</v>
       </c>
     </row>
@@ -401,89 +407,89 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="2" t="n">
         <v>400</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8" s="2" t="n">
         <v>416</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="2" t="n">
         <v>432</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="E8" s="2" t="n">
         <v>272</v>
       </c>
-      <c r="F8" s="0" t="n">
+      <c r="F8" s="2" t="n">
         <v>384</v>
       </c>
-      <c r="G8" s="0" t="n">
+      <c r="G8" s="2" t="n">
         <v>272</v>
       </c>
-      <c r="H8" s="0" t="n">
+      <c r="H8" s="2" t="n">
         <v>544</v>
       </c>
-      <c r="I8" s="0" t="n">
+      <c r="I8" s="2" t="n">
         <v>352</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B9" s="2" t="n">
         <v>240</v>
       </c>
-      <c r="C9" s="0" t="n">
+      <c r="C9" s="2" t="n">
         <v>176</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="D9" s="2" t="n">
         <v>-241</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="E9" s="2" t="n">
         <v>-224</v>
       </c>
-      <c r="F9" s="0" t="n">
+      <c r="F9" s="2" t="n">
         <v>96</v>
       </c>
-      <c r="G9" s="0" t="n">
+      <c r="G9" s="2" t="n">
         <v>240</v>
       </c>
-      <c r="H9" s="0" t="n">
+      <c r="H9" s="2" t="n">
         <v>368</v>
       </c>
-      <c r="I9" s="0" t="n">
+      <c r="I9" s="2" t="n">
         <v>320</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10" s="2" t="n">
         <v>-448</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="C10" s="2" t="n">
         <v>-336</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="D10" s="2" t="n">
         <v>-192</v>
       </c>
-      <c r="E10" s="0" t="n">
+      <c r="E10" s="2" t="n">
         <v>-128</v>
       </c>
-      <c r="F10" s="0" t="n">
+      <c r="F10" s="2" t="n">
         <v>-400</v>
       </c>
-      <c r="G10" s="0" t="n">
+      <c r="G10" s="2" t="n">
         <v>-208</v>
       </c>
-      <c r="H10" s="0" t="n">
+      <c r="H10" s="2" t="n">
         <v>-32</v>
       </c>
-      <c r="I10" s="0" t="n">
+      <c r="I10" s="2" t="n">
         <v>-640</v>
       </c>
     </row>
@@ -493,115 +499,151 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="0" t="n">
+      <c r="B14" s="2" t="n">
         <f aca="false">B8*0.049</f>
         <v>19.6</v>
       </c>
-      <c r="C14" s="0" t="n">
+      <c r="C14" s="2" t="n">
         <f aca="false">C8*0.049</f>
         <v>20.384</v>
       </c>
-      <c r="D14" s="0" t="n">
+      <c r="D14" s="2" t="n">
         <f aca="false">D8*0.049</f>
         <v>21.168</v>
       </c>
-      <c r="E14" s="0" t="n">
+      <c r="E14" s="2" t="n">
         <f aca="false">E8*0.049</f>
         <v>13.328</v>
       </c>
-      <c r="F14" s="0" t="n">
+      <c r="F14" s="2" t="n">
         <f aca="false">F8*0.049</f>
         <v>18.816</v>
       </c>
-      <c r="G14" s="0" t="n">
+      <c r="G14" s="2" t="n">
         <f aca="false">G8*0.049</f>
         <v>13.328</v>
       </c>
-      <c r="H14" s="0" t="n">
+      <c r="H14" s="2" t="n">
         <f aca="false">H8*0.049</f>
         <v>26.656</v>
       </c>
-      <c r="I14" s="0" t="n">
+      <c r="I14" s="2" t="n">
         <f aca="false">I8*0.049</f>
         <v>17.248</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="0" t="n">
+      <c r="B15" s="2" t="n">
         <f aca="false">B9*0.049</f>
         <v>11.76</v>
       </c>
-      <c r="C15" s="0" t="n">
+      <c r="C15" s="2" t="n">
         <f aca="false">C9*0.049</f>
         <v>8.624</v>
       </c>
-      <c r="D15" s="0" t="n">
+      <c r="D15" s="2" t="n">
         <f aca="false">D9*0.049</f>
         <v>-11.809</v>
       </c>
-      <c r="E15" s="0" t="n">
+      <c r="E15" s="2" t="n">
         <f aca="false">E9*0.049</f>
         <v>-10.976</v>
       </c>
-      <c r="F15" s="0" t="n">
+      <c r="F15" s="2" t="n">
         <f aca="false">F9*0.049</f>
         <v>4.704</v>
       </c>
-      <c r="G15" s="0" t="n">
+      <c r="G15" s="2" t="n">
         <f aca="false">G9*0.049</f>
         <v>11.76</v>
       </c>
-      <c r="H15" s="0" t="n">
+      <c r="H15" s="2" t="n">
         <f aca="false">H9*0.049</f>
         <v>18.032</v>
       </c>
-      <c r="I15" s="0" t="n">
+      <c r="I15" s="2" t="n">
         <f aca="false">I9*0.049</f>
         <v>15.68</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="0" t="n">
+      <c r="B16" s="2" t="n">
         <f aca="false">B10*0.049</f>
         <v>-21.952</v>
       </c>
-      <c r="C16" s="0" t="n">
+      <c r="C16" s="2" t="n">
         <f aca="false">C10*0.049</f>
         <v>-16.464</v>
       </c>
-      <c r="D16" s="0" t="n">
+      <c r="D16" s="2" t="n">
         <f aca="false">D10*0.049</f>
         <v>-9.408</v>
       </c>
-      <c r="E16" s="0" t="n">
+      <c r="E16" s="2" t="n">
         <f aca="false">E10*0.049</f>
         <v>-6.272</v>
       </c>
-      <c r="F16" s="0" t="n">
+      <c r="F16" s="2" t="n">
         <f aca="false">F10*0.049</f>
         <v>-19.6</v>
       </c>
-      <c r="G16" s="0" t="n">
+      <c r="G16" s="2" t="n">
         <f aca="false">G10*0.049</f>
         <v>-10.192</v>
       </c>
-      <c r="H16" s="0" t="n">
+      <c r="H16" s="2" t="n">
         <f aca="false">H10*0.049</f>
         <v>-1.568</v>
       </c>
-      <c r="I16" s="0" t="n">
+      <c r="I16" s="2" t="n">
         <f aca="false">I10*0.049</f>
         <v>-31.36</v>
       </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>